<commit_message>
Create fun for com, subcom and unit added
</commit_message>
<xml_diff>
--- a/BraasiDB.xlsx
+++ b/BraasiDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana\moje\programovani\Braasi\braasi_desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F63756-76C2-477B-9AF5-998F5A90BCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7762825D-118A-45F5-9C2C-83B37716034E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stock_on_hand" sheetId="3" r:id="rId1"/>
@@ -2483,8 +2483,8 @@
   </sheetPr>
   <dimension ref="A1:E1150"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13069,14 +13069,14 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B4D40F-943B-4A09-A4D8-F1D19899B5FB}">
-  <sheetPr codeName="Sheet4">
+  <sheetPr codeName="Sheet4" filterMode="1">
     <tabColor rgb="FF92D050"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E584"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13117,7 +13117,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -13132,7 +13132,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -13147,7 +13147,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -13177,7 +13177,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -13192,7 +13192,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
@@ -13222,7 +13222,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -13237,7 +13237,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>69</v>
       </c>
@@ -13252,7 +13252,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
@@ -13267,7 +13267,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>73</v>
       </c>
@@ -13282,7 +13282,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
@@ -13297,7 +13297,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>77</v>
       </c>
@@ -13312,7 +13312,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -13327,7 +13327,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
@@ -13342,7 +13342,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
@@ -13357,7 +13357,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
@@ -13372,7 +13372,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>87</v>
       </c>
@@ -13387,7 +13387,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
@@ -13402,7 +13402,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>91</v>
       </c>
@@ -13417,7 +13417,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>93</v>
       </c>
@@ -13432,7 +13432,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>95</v>
       </c>
@@ -13447,7 +13447,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
@@ -13462,7 +13462,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
@@ -13477,7 +13477,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>101</v>
       </c>
@@ -13492,7 +13492,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>103</v>
       </c>
@@ -13507,7 +13507,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>105</v>
       </c>
@@ -13522,7 +13522,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -13537,7 +13537,7 @@
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>109</v>
       </c>
@@ -13552,7 +13552,7 @@
       </c>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>111</v>
       </c>
@@ -13567,7 +13567,7 @@
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>113</v>
       </c>
@@ -13582,7 +13582,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>115</v>
       </c>
@@ -13597,7 +13597,7 @@
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>117</v>
       </c>
@@ -13612,7 +13612,7 @@
       </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>119</v>
       </c>
@@ -13627,7 +13627,7 @@
       </c>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>121</v>
       </c>
@@ -13642,7 +13642,7 @@
       </c>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>123</v>
       </c>
@@ -13657,7 +13657,7 @@
       </c>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>125</v>
       </c>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>127</v>
       </c>
@@ -13687,7 +13687,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>129</v>
       </c>
@@ -13702,7 +13702,7 @@
       </c>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>131</v>
       </c>
@@ -13717,7 +13717,7 @@
       </c>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>133</v>
       </c>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>135</v>
       </c>
@@ -13747,7 +13747,7 @@
       </c>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>137</v>
       </c>
@@ -13762,7 +13762,7 @@
       </c>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>139</v>
       </c>
@@ -13777,7 +13777,7 @@
       </c>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>141</v>
       </c>
@@ -13792,7 +13792,7 @@
       </c>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>143</v>
       </c>
@@ -13807,7 +13807,7 @@
       </c>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>145</v>
       </c>
@@ -13822,7 +13822,7 @@
       </c>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -13837,7 +13837,7 @@
       </c>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>149</v>
       </c>
@@ -13852,7 +13852,7 @@
       </c>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>151</v>
       </c>
@@ -13867,7 +13867,7 @@
       </c>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>153</v>
       </c>
@@ -13882,7 +13882,7 @@
       </c>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>155</v>
       </c>
@@ -13897,7 +13897,7 @@
       </c>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>157</v>
       </c>
@@ -13912,7 +13912,7 @@
       </c>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>159</v>
       </c>
@@ -13927,7 +13927,7 @@
       </c>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>161</v>
       </c>
@@ -13942,7 +13942,7 @@
       </c>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>163</v>
       </c>
@@ -13957,7 +13957,7 @@
       </c>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>165</v>
       </c>
@@ -13972,7 +13972,7 @@
       </c>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>167</v>
       </c>
@@ -13987,7 +13987,7 @@
       </c>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>169</v>
       </c>
@@ -14002,7 +14002,7 @@
       </c>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>15</v>
       </c>
@@ -14017,7 +14017,7 @@
       </c>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>18</v>
       </c>
@@ -14032,7 +14032,7 @@
       </c>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>171</v>
       </c>
@@ -14047,7 +14047,7 @@
       </c>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>173</v>
       </c>
@@ -14062,7 +14062,7 @@
       </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>175</v>
       </c>
@@ -14077,7 +14077,7 @@
       </c>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -14092,7 +14092,7 @@
       </c>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>177</v>
       </c>
@@ -14107,7 +14107,7 @@
       </c>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>179</v>
       </c>
@@ -14122,7 +14122,7 @@
       </c>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>181</v>
       </c>
@@ -14137,7 +14137,7 @@
       </c>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>183</v>
       </c>
@@ -14152,7 +14152,7 @@
       </c>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>185</v>
       </c>
@@ -14167,7 +14167,7 @@
       </c>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>187</v>
       </c>
@@ -14182,7 +14182,7 @@
       </c>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>189</v>
       </c>
@@ -14197,7 +14197,7 @@
       </c>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>22</v>
       </c>
@@ -14212,7 +14212,7 @@
       </c>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>24</v>
       </c>
@@ -14227,7 +14227,7 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>191</v>
       </c>
@@ -14242,7 +14242,7 @@
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>193</v>
       </c>
@@ -14257,7 +14257,7 @@
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>195</v>
       </c>
@@ -14272,7 +14272,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>197</v>
       </c>
@@ -14287,7 +14287,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>199</v>
       </c>
@@ -14302,7 +14302,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>201</v>
       </c>
@@ -14317,7 +14317,7 @@
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>203</v>
       </c>
@@ -14332,7 +14332,7 @@
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>205</v>
       </c>
@@ -14347,7 +14347,7 @@
       </c>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>207</v>
       </c>
@@ -14362,7 +14362,7 @@
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>209</v>
       </c>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>211</v>
       </c>
@@ -14392,7 +14392,7 @@
       </c>
       <c r="E87" s="2"/>
     </row>
-    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>213</v>
       </c>
@@ -14407,7 +14407,7 @@
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>215</v>
       </c>
@@ -14422,7 +14422,7 @@
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>217</v>
       </c>
@@ -14437,7 +14437,7 @@
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>219</v>
       </c>
@@ -14452,7 +14452,7 @@
       </c>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>221</v>
       </c>
@@ -14467,7 +14467,7 @@
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>223</v>
       </c>
@@ -14482,7 +14482,7 @@
       </c>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>225</v>
       </c>
@@ -14497,7 +14497,7 @@
       </c>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>227</v>
       </c>
@@ -14512,7 +14512,7 @@
       </c>
       <c r="E95" s="2"/>
     </row>
-    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>229</v>
       </c>
@@ -14527,7 +14527,7 @@
       </c>
       <c r="E96" s="2"/>
     </row>
-    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>231</v>
       </c>
@@ -14542,7 +14542,7 @@
       </c>
       <c r="E97" s="2"/>
     </row>
-    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>233</v>
       </c>
@@ -14557,7 +14557,7 @@
       </c>
       <c r="E98" s="2"/>
     </row>
-    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>235</v>
       </c>
@@ -14572,7 +14572,7 @@
       </c>
       <c r="E99" s="2"/>
     </row>
-    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>237</v>
       </c>
@@ -14587,7 +14587,7 @@
       </c>
       <c r="E100" s="2"/>
     </row>
-    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>239</v>
       </c>
@@ -14602,7 +14602,7 @@
       </c>
       <c r="E101" s="2"/>
     </row>
-    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>241</v>
       </c>
@@ -14617,7 +14617,7 @@
       </c>
       <c r="E102" s="2"/>
     </row>
-    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>243</v>
       </c>
@@ -14632,7 +14632,7 @@
       </c>
       <c r="E103" s="2"/>
     </row>
-    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>245</v>
       </c>
@@ -14647,7 +14647,7 @@
       </c>
       <c r="E104" s="2"/>
     </row>
-    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>247</v>
       </c>
@@ -14662,7 +14662,7 @@
       </c>
       <c r="E105" s="2"/>
     </row>
-    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>249</v>
       </c>
@@ -14677,7 +14677,7 @@
       </c>
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>251</v>
       </c>
@@ -14692,7 +14692,7 @@
       </c>
       <c r="E107" s="2"/>
     </row>
-    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>253</v>
       </c>
@@ -14707,7 +14707,7 @@
       </c>
       <c r="E108" s="2"/>
     </row>
-    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>255</v>
       </c>
@@ -14722,7 +14722,7 @@
       </c>
       <c r="E109" s="2"/>
     </row>
-    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>257</v>
       </c>
@@ -14737,7 +14737,7 @@
       </c>
       <c r="E110" s="2"/>
     </row>
-    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>259</v>
       </c>
@@ -14752,7 +14752,7 @@
       </c>
       <c r="E111" s="2"/>
     </row>
-    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>261</v>
       </c>
@@ -14767,7 +14767,7 @@
       </c>
       <c r="E112" s="2"/>
     </row>
-    <row r="113" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>263</v>
       </c>
@@ -14782,7 +14782,7 @@
       </c>
       <c r="E113" s="2"/>
     </row>
-    <row r="114" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>265</v>
       </c>
@@ -14797,7 +14797,7 @@
       </c>
       <c r="E114" s="2"/>
     </row>
-    <row r="115" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>267</v>
       </c>
@@ -14812,7 +14812,7 @@
       </c>
       <c r="E115" s="2"/>
     </row>
-    <row r="116" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>269</v>
       </c>
@@ -14827,7 +14827,7 @@
       </c>
       <c r="E116" s="2"/>
     </row>
-    <row r="117" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>271</v>
       </c>
@@ -14842,7 +14842,7 @@
       </c>
       <c r="E117" s="2"/>
     </row>
-    <row r="118" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>273</v>
       </c>
@@ -14857,7 +14857,7 @@
       </c>
       <c r="E118" s="2"/>
     </row>
-    <row r="119" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>275</v>
       </c>
@@ -14872,7 +14872,7 @@
       </c>
       <c r="E119" s="2"/>
     </row>
-    <row r="120" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>277</v>
       </c>
@@ -14887,7 +14887,7 @@
       </c>
       <c r="E120" s="2"/>
     </row>
-    <row r="121" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>279</v>
       </c>
@@ -14902,7 +14902,7 @@
       </c>
       <c r="E121" s="2"/>
     </row>
-    <row r="122" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>281</v>
       </c>
@@ -14917,7 +14917,7 @@
       </c>
       <c r="E122" s="2"/>
     </row>
-    <row r="123" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>283</v>
       </c>
@@ -14932,7 +14932,7 @@
       </c>
       <c r="E123" s="2"/>
     </row>
-    <row r="124" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>285</v>
       </c>
@@ -14947,7 +14947,7 @@
       </c>
       <c r="E124" s="2"/>
     </row>
-    <row r="125" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>287</v>
       </c>
@@ -14962,7 +14962,7 @@
       </c>
       <c r="E125" s="2"/>
     </row>
-    <row r="126" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>289</v>
       </c>
@@ -14977,7 +14977,7 @@
       </c>
       <c r="E126" s="2"/>
     </row>
-    <row r="127" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>291</v>
       </c>
@@ -14992,7 +14992,7 @@
       </c>
       <c r="E127" s="2"/>
     </row>
-    <row r="128" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>293</v>
       </c>
@@ -15007,7 +15007,7 @@
       </c>
       <c r="E128" s="2"/>
     </row>
-    <row r="129" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>295</v>
       </c>
@@ -15022,7 +15022,7 @@
       </c>
       <c r="E129" s="2"/>
     </row>
-    <row r="130" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>297</v>
       </c>
@@ -15037,7 +15037,7 @@
       </c>
       <c r="E130" s="2"/>
     </row>
-    <row r="131" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>299</v>
       </c>
@@ -15052,7 +15052,7 @@
       </c>
       <c r="E131" s="2"/>
     </row>
-    <row r="132" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>301</v>
       </c>
@@ -15067,7 +15067,7 @@
       </c>
       <c r="E132" s="2"/>
     </row>
-    <row r="133" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>303</v>
       </c>
@@ -15082,7 +15082,7 @@
       </c>
       <c r="E133" s="2"/>
     </row>
-    <row r="134" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>305</v>
       </c>
@@ -15097,7 +15097,7 @@
       </c>
       <c r="E134" s="2"/>
     </row>
-    <row r="135" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>307</v>
       </c>
@@ -15112,7 +15112,7 @@
       </c>
       <c r="E135" s="2"/>
     </row>
-    <row r="136" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>309</v>
       </c>
@@ -15127,7 +15127,7 @@
       </c>
       <c r="E136" s="2"/>
     </row>
-    <row r="137" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>311</v>
       </c>
@@ -15142,7 +15142,7 @@
       </c>
       <c r="E137" s="2"/>
     </row>
-    <row r="138" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>313</v>
       </c>
@@ -15157,7 +15157,7 @@
       </c>
       <c r="E138" s="2"/>
     </row>
-    <row r="139" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>315</v>
       </c>
@@ -15174,7 +15174,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>317</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>319</v>
       </c>
@@ -15208,7 +15208,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>321</v>
       </c>
@@ -15225,7 +15225,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>323</v>
       </c>
@@ -15242,7 +15242,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>325</v>
       </c>
@@ -15259,7 +15259,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>327</v>
       </c>
@@ -15276,7 +15276,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>26</v>
       </c>
@@ -15293,7 +15293,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>329</v>
       </c>
@@ -15310,7 +15310,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>29</v>
       </c>
@@ -15325,7 +15325,7 @@
       </c>
       <c r="E148" s="2"/>
     </row>
-    <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>331</v>
       </c>
@@ -15340,7 +15340,7 @@
       </c>
       <c r="E149" s="2"/>
     </row>
-    <row r="150" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>333</v>
       </c>
@@ -15355,7 +15355,7 @@
       </c>
       <c r="E150" s="2"/>
     </row>
-    <row r="151" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>335</v>
       </c>
@@ -15370,7 +15370,7 @@
       </c>
       <c r="E151" s="2"/>
     </row>
-    <row r="152" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>337</v>
       </c>
@@ -15385,7 +15385,7 @@
       </c>
       <c r="E152" s="2"/>
     </row>
-    <row r="153" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>339</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>341</v>
       </c>
@@ -15419,7 +15419,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>343</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>345</v>
       </c>
@@ -15453,7 +15453,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>36</v>
       </c>
@@ -15470,7 +15470,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>347</v>
       </c>
@@ -15487,7 +15487,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>349</v>
       </c>
@@ -15504,7 +15504,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>351</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>353</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>355</v>
       </c>
@@ -15555,7 +15555,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>357</v>
       </c>
@@ -15572,7 +15572,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>359</v>
       </c>
@@ -15589,7 +15589,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>361</v>
       </c>
@@ -15606,7 +15606,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>363</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>365</v>
       </c>
@@ -15640,7 +15640,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>367</v>
       </c>
@@ -15657,7 +15657,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>369</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>371</v>
       </c>
@@ -15691,7 +15691,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>373</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>375</v>
       </c>
@@ -15725,7 +15725,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>377</v>
       </c>
@@ -15742,7 +15742,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>379</v>
       </c>
@@ -15759,7 +15759,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>381</v>
       </c>
@@ -15776,7 +15776,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>383</v>
       </c>
@@ -15793,7 +15793,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>385</v>
       </c>
@@ -15810,7 +15810,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>387</v>
       </c>
@@ -15827,7 +15827,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>389</v>
       </c>
@@ -15844,7 +15844,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>391</v>
       </c>
@@ -15861,7 +15861,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>393</v>
       </c>
@@ -15878,7 +15878,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>395</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>397</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>399</v>
       </c>
@@ -15929,7 +15929,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>401</v>
       </c>
@@ -15946,7 +15946,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>403</v>
       </c>
@@ -15963,7 +15963,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>405</v>
       </c>
@@ -15980,7 +15980,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>407</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>409</v>
       </c>
@@ -16014,7 +16014,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>411</v>
       </c>
@@ -16031,7 +16031,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>413</v>
       </c>
@@ -16048,7 +16048,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>415</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>417</v>
       </c>
@@ -16082,7 +16082,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>419</v>
       </c>
@@ -16099,7 +16099,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>421</v>
       </c>
@@ -16116,7 +16116,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>423</v>
       </c>
@@ -16133,7 +16133,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>425</v>
       </c>
@@ -16150,7 +16150,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>427</v>
       </c>
@@ -16167,7 +16167,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>429</v>
       </c>
@@ -16184,7 +16184,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>431</v>
       </c>
@@ -16201,7 +16201,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>433</v>
       </c>
@@ -16218,7 +16218,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>435</v>
       </c>
@@ -16235,7 +16235,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>437</v>
       </c>
@@ -16252,7 +16252,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>439</v>
       </c>
@@ -16269,7 +16269,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>441</v>
       </c>
@@ -16286,7 +16286,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>443</v>
       </c>
@@ -16303,7 +16303,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>445</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>447</v>
       </c>
@@ -16337,7 +16337,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>449</v>
       </c>
@@ -16354,7 +16354,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>451</v>
       </c>
@@ -16371,7 +16371,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>453</v>
       </c>
@@ -16388,7 +16388,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>455</v>
       </c>
@@ -16405,7 +16405,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>457</v>
       </c>
@@ -16422,7 +16422,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>459</v>
       </c>
@@ -16439,7 +16439,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>461</v>
       </c>
@@ -16456,7 +16456,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>463</v>
       </c>
@@ -16473,7 +16473,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>465</v>
       </c>
@@ -16490,7 +16490,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>467</v>
       </c>
@@ -16507,7 +16507,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>469</v>
       </c>
@@ -16524,7 +16524,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>471</v>
       </c>
@@ -16541,7 +16541,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>473</v>
       </c>
@@ -16558,7 +16558,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>475</v>
       </c>
@@ -16575,7 +16575,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>477</v>
       </c>
@@ -16592,7 +16592,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>479</v>
       </c>
@@ -16609,7 +16609,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>481</v>
       </c>
@@ -16626,7 +16626,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>483</v>
       </c>
@@ -16643,7 +16643,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>485</v>
       </c>
@@ -16660,7 +16660,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>487</v>
       </c>
@@ -16677,7 +16677,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>489</v>
       </c>
@@ -16694,7 +16694,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>491</v>
       </c>
@@ -16711,7 +16711,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>493</v>
       </c>
@@ -16728,7 +16728,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>34</v>
       </c>
@@ -16745,7 +16745,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>495</v>
       </c>
@@ -16762,7 +16762,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>497</v>
       </c>
@@ -16779,7 +16779,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>499</v>
       </c>
@@ -16796,7 +16796,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>501</v>
       </c>
@@ -16813,7 +16813,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>503</v>
       </c>
@@ -16830,7 +16830,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
         <v>505</v>
       </c>
@@ -16847,7 +16847,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>507</v>
       </c>
@@ -16864,7 +16864,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>509</v>
       </c>
@@ -16881,7 +16881,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>511</v>
       </c>
@@ -16898,7 +16898,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
         <v>513</v>
       </c>
@@ -16915,7 +16915,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>32</v>
       </c>
@@ -17202,7 +17202,7 @@
       </c>
       <c r="E261" s="2"/>
     </row>
-    <row r="262" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
         <v>38</v>
       </c>
@@ -17219,7 +17219,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="263" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>547</v>
       </c>
@@ -17236,7 +17236,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
         <v>549</v>
       </c>
@@ -17253,7 +17253,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
         <v>551</v>
       </c>
@@ -17270,7 +17270,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
         <v>553</v>
       </c>
@@ -17287,7 +17287,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
         <v>555</v>
       </c>
@@ -17304,7 +17304,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
         <v>557</v>
       </c>
@@ -17319,7 +17319,7 @@
       </c>
       <c r="E268" s="2"/>
     </row>
-    <row r="269" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
         <v>559</v>
       </c>
@@ -17334,7 +17334,7 @@
       </c>
       <c r="E269" s="2"/>
     </row>
-    <row r="270" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
         <v>561</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
         <v>563</v>
       </c>
@@ -17366,7 +17366,7 @@
       </c>
       <c r="E271" s="2"/>
     </row>
-    <row r="272" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
         <v>565</v>
       </c>
@@ -17381,7 +17381,7 @@
       </c>
       <c r="E272" s="2"/>
     </row>
-    <row r="273" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
         <v>567</v>
       </c>
@@ -17396,7 +17396,7 @@
       </c>
       <c r="E273" s="2"/>
     </row>
-    <row r="274" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
         <v>569</v>
       </c>
@@ -17411,7 +17411,7 @@
       </c>
       <c r="E274" s="2"/>
     </row>
-    <row r="275" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>571</v>
       </c>
@@ -17426,7 +17426,7 @@
       </c>
       <c r="E275" s="2"/>
     </row>
-    <row r="276" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
         <v>573</v>
       </c>
@@ -17441,7 +17441,7 @@
       </c>
       <c r="E276" s="2"/>
     </row>
-    <row r="277" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>575</v>
       </c>
@@ -17456,7 +17456,7 @@
       </c>
       <c r="E277" s="2"/>
     </row>
-    <row r="278" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
         <v>577</v>
       </c>
@@ -17471,7 +17471,7 @@
       </c>
       <c r="E278" s="2"/>
     </row>
-    <row r="279" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
         <v>579</v>
       </c>
@@ -17486,7 +17486,7 @@
       </c>
       <c r="E279" s="2"/>
     </row>
-    <row r="280" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
         <v>581</v>
       </c>
@@ -17501,7 +17501,7 @@
       </c>
       <c r="E280" s="2"/>
     </row>
-    <row r="281" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
         <v>583</v>
       </c>
@@ -17516,7 +17516,7 @@
       </c>
       <c r="E281" s="2"/>
     </row>
-    <row r="282" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>585</v>
       </c>
@@ -17531,7 +17531,7 @@
       </c>
       <c r="E282" s="2"/>
     </row>
-    <row r="283" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>587</v>
       </c>
@@ -17546,7 +17546,7 @@
       </c>
       <c r="E283" s="2"/>
     </row>
-    <row r="284" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
         <v>589</v>
       </c>
@@ -17561,7 +17561,7 @@
       </c>
       <c r="E284" s="2"/>
     </row>
-    <row r="285" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>591</v>
       </c>
@@ -17576,7 +17576,7 @@
       </c>
       <c r="E285" s="2"/>
     </row>
-    <row r="286" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
         <v>593</v>
       </c>
@@ -17591,7 +17591,7 @@
       </c>
       <c r="E286" s="2"/>
     </row>
-    <row r="287" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
         <v>595</v>
       </c>
@@ -17606,7 +17606,7 @@
       </c>
       <c r="E287" s="2"/>
     </row>
-    <row r="288" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="2" t="s">
         <v>40</v>
       </c>
@@ -17621,7 +17621,7 @@
       </c>
       <c r="E288" s="2"/>
     </row>
-    <row r="289" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
         <v>43</v>
       </c>
@@ -17636,7 +17636,7 @@
       </c>
       <c r="E289" s="2"/>
     </row>
-    <row r="290" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="2" t="s">
         <v>45</v>
       </c>
@@ -17651,7 +17651,7 @@
       </c>
       <c r="E290" s="2"/>
     </row>
-    <row r="291" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
         <v>47</v>
       </c>
@@ -17666,7 +17666,7 @@
       </c>
       <c r="E291" s="2"/>
     </row>
-    <row r="292" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
         <v>51</v>
       </c>
@@ -17681,7 +17681,7 @@
       </c>
       <c r="E292" s="2"/>
     </row>
-    <row r="293" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="2" t="s">
         <v>49</v>
       </c>
@@ -19734,7 +19734,13 @@
       <c r="E584" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E293" xr:uid="{B0B4D40F-943B-4A09-A4D8-F1D19899B5FB}"/>
+  <autoFilter ref="A2:E293" xr:uid="{B0B4D40F-943B-4A09-A4D8-F1D19899B5FB}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="BRA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -30704,7 +30710,7 @@
   <dimension ref="A1:H1002"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35808,7 +35814,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EDFA39-F887-4FCF-A865-B3FAD130D22C}">
-  <sheetPr>
+  <sheetPr codeName="Sheet11">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C13"/>

</xml_diff>